<commit_message>
Fix to contain type key when type check
</commit_message>
<xml_diff>
--- a/Sample/HelloExcelToMySql/Excel/Sample.xlsx
+++ b/Sample/HelloExcelToMySql/Excel/Sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkspaceGit\ExcelToMySql\Sample\HelloExcelToMySql\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,35 +26,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>short</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>char</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>this_is_text</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ref</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>this_is_ref</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int_column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>column_short</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char_column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>column_byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text_column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>column_ref</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -422,29 +422,29 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -461,10 +461,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>